<commit_message>
v1.12 - e2e Testing
</commit_message>
<xml_diff>
--- a/test/assets/valid_rcm.xlsx
+++ b/test/assets/valid_rcm.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,17 +471,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P-TEST-01</t>
+          <t>ITGC-OP-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>발주 승인</t>
+          <t>테스트 접근권한 관리</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>발주 승인 설명</t>
+          <t>시스템 접근 권한을 적절히 부여하고 관리한다.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>일</t>
+          <t>상시</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -506,59 +506,106 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>모집단 설명</t>
+          <t>접근권한 목록</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>테스트 절차</t>
+          <t>권한 부여 현황 확인</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P-TEST-02</t>
+          <t>ITGC-OP-02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>입고 확인</t>
+          <t>테스트 변경관리</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>입고 확인 설명</t>
+          <t>시스템 변경 시 승인 절차를 따른다.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>수시</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>탐지</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>자동</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>변경요청서</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>변경 승인 이력 확인</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ITGC-OP-03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>테스트 운영 보안</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>운영 환경의 보안을 유지한다.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>N</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>주</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>적발</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>자동</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>모집단 설명2</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>테스트 절차2</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>월별</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>예방</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>수동</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>보안점검표</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>월별 점검 결과 확인</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.13 - Unit Test
</commit_message>
<xml_diff>
--- a/test/assets/valid_rcm.xlsx
+++ b/test/assets/valid_rcm.xlsx
@@ -471,7 +471,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ITGC-OP-01</t>
+          <t>ITGC-TEST-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ITGC-OP-02</t>
+          <t>ITGC-TEST-02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -565,7 +565,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ITGC-OP-03</t>
+          <t>ITGC-TEST-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>

<commit_message>
v1.14 - Unit Test Complete
</commit_message>
<xml_diff>
--- a/test/assets/valid_rcm.xlsx
+++ b/test/assets/valid_rcm.xlsx
@@ -471,7 +471,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ITGC-TEST-01</t>
+          <t>ITGC-OP-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -518,7 +518,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ITGC-TEST-02</t>
+          <t>ITGC-OP-02</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -565,7 +565,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ITGC-TEST-03</t>
+          <t>ITGC-OP-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">

</xml_diff>